<commit_message>
Addition of Excel Project README
</commit_message>
<xml_diff>
--- a/excel/Curso DIO - Dashboard interativo de vendas do xbox/dashboard_xbox.xlsx
+++ b/excel/Curso DIO - Dashboard interativo de vendas do xbox/dashboard_xbox.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\RPG\Portfolio\excel\Curso DIO - Dashboard interativo de vendas do xbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C6F185-8079-4F6E-9A4F-F8ADF3895FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16686203-B9ED-4E78-A321-E82B9812F30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
   <sheets>
-    <sheet name="A̳ssets" sheetId="1" r:id="rId1"/>
-    <sheet name="B̳ases" sheetId="2" r:id="rId2"/>
-    <sheet name="C̳álculos" sheetId="3" r:id="rId3"/>
+    <sheet name="A̳ssets" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="B̳ases" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="C̳álculos" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="D̳ashboard" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -1161,7 +1161,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1191,7 +1191,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -12627,7 +12626,7 @@
   <dimension ref="B3:P21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12800,7 +12799,7 @@
   <dimension ref="A1:M296"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25058,7 +25057,7 @@
       <c r="A21" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21">
         <v>0</v>
       </c>
     </row>
@@ -25066,7 +25065,7 @@
       <c r="A22" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22">
         <v>0</v>
       </c>
     </row>
@@ -25074,7 +25073,7 @@
       <c r="A23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23">
         <v>600</v>
       </c>
       <c r="D23" s="16">
@@ -25087,7 +25086,7 @@
       <c r="A24" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24">
         <v>600</v>
       </c>
     </row>
@@ -25243,16 +25242,16 @@
       <c r="A65" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B65" s="19">
+      <c r="B65">
         <v>5</v>
       </c>
-      <c r="C65" s="19">
+      <c r="C65">
         <v>4</v>
       </c>
-      <c r="D65" s="19">
+      <c r="D65">
         <v>2</v>
       </c>
-      <c r="E65" s="19">
+      <c r="E65">
         <v>11</v>
       </c>
     </row>
@@ -25260,16 +25259,16 @@
       <c r="A66" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B66" s="19">
+      <c r="B66">
         <v>19</v>
       </c>
-      <c r="C66" s="19">
+      <c r="C66">
         <v>23</v>
       </c>
-      <c r="D66" s="19">
+      <c r="D66">
         <v>18</v>
       </c>
-      <c r="E66" s="19">
+      <c r="E66">
         <v>60</v>
       </c>
     </row>
@@ -25277,16 +25276,16 @@
       <c r="A67" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="B67" s="19">
+      <c r="B67">
         <v>24</v>
       </c>
-      <c r="C67" s="19">
+      <c r="C67">
         <v>27</v>
       </c>
-      <c r="D67" s="19">
+      <c r="D67">
         <v>20</v>
       </c>
-      <c r="E67" s="19">
+      <c r="E67">
         <v>71</v>
       </c>
     </row>
@@ -48244,26 +48243,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010001E48B58A68BE64E9120D347E3E06B3A" ma:contentTypeVersion="19" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2f90046ec77328b7f86417d2e03b3d33">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851b35d3-0456-4d6a-bc2f-da927e91d158" xmlns:ns3="19483571-f922-4e8e-9c1c-26f0a2252132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c815006ac2d4f05ee97fdd57e40d8e38" ns2:_="" ns3:_="">
     <xsd:import namespace="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
@@ -48518,10 +48497,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32608D25-EC36-42FE-A1DC-F778995A6799}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
+    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -48538,20 +48548,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32608D25-EC36-42FE-A1DC-F778995A6799}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
-    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>